<commit_message>
Merged all of the files in common/technologies
Fixed some other stuff as well
</commit_message>
<xml_diff>
--- a/Need to be Merged.xlsx
+++ b/Need to be Merged.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dante\Documents\Paradox Interactive\Hearts of Iron IV\mod\1984DEV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC2BEDA-F00E-4109-B709-21549E4CB53E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BDDF9E-A2A1-4F09-8005-549CD2B35C69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="6855" windowWidth="26085" windowHeight="11535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2100" yWindow="3120" windowWidth="26085" windowHeight="13110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
   <si>
     <t>industry.txt</t>
   </si>
@@ -135,6 +135,105 @@
   </si>
   <si>
     <t>Equipment</t>
+  </si>
+  <si>
+    <t>Common Technologies</t>
+  </si>
+  <si>
+    <t>Localization</t>
+  </si>
+  <si>
+    <t>stats_l_english.yml</t>
+  </si>
+  <si>
+    <t>technology_sharing_l_english.yml</t>
+  </si>
+  <si>
+    <t>traits_l_english.yml</t>
+  </si>
+  <si>
+    <t>unit_l_english.yml</t>
+  </si>
+  <si>
+    <t>victory_points_l_english.yml</t>
+  </si>
+  <si>
+    <t>war_l_english.yml</t>
+  </si>
+  <si>
+    <t>bookmarks_l_english.yml</t>
+  </si>
+  <si>
+    <t>countries_cosmetic_l_english.yml</t>
+  </si>
+  <si>
+    <t>countries_l_english.yml</t>
+  </si>
+  <si>
+    <t>equip_air_l_english.yml</t>
+  </si>
+  <si>
+    <t>equip_naval_l_english.yml</t>
+  </si>
+  <si>
+    <t>equipment_l_english.yml</t>
+  </si>
+  <si>
+    <t>events_l_english.yml</t>
+  </si>
+  <si>
+    <t>frontend_l_english.yml</t>
+  </si>
+  <si>
+    <t>ideas_l_english.yml</t>
+  </si>
+  <si>
+    <t>loading_tips_l_english.yml</t>
+  </si>
+  <si>
+    <t>modifiers_l_english.yml</t>
+  </si>
+  <si>
+    <t>nef_council_l_english.yml</t>
+  </si>
+  <si>
+    <t>nef_despdefense_l_english.yml</t>
+  </si>
+  <si>
+    <t>nef_eventcountry_l_english.yml</t>
+  </si>
+  <si>
+    <t>nef_eventelection_l_english.yml</t>
+  </si>
+  <si>
+    <t>nef_eventnews_l_english.yml</t>
+  </si>
+  <si>
+    <t>nef_factions_l_english.yml</t>
+  </si>
+  <si>
+    <t>nef_focus_resistance_l_english.yml</t>
+  </si>
+  <si>
+    <t>nef_focus_totalitarian_l_english.yml</t>
+  </si>
+  <si>
+    <t>nef_ideas_l_english.yml</t>
+  </si>
+  <si>
+    <t>nef_other_l_english.yml</t>
+  </si>
+  <si>
+    <t>parties_l_english.yml</t>
+  </si>
+  <si>
+    <t>research_l_english.yml</t>
+  </si>
+  <si>
+    <t>state_names_l_english.yml</t>
+  </si>
+  <si>
+    <t>Didn’t need to</t>
   </si>
 </sst>
 </file>
@@ -200,12 +299,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,17 +598,14 @@
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>11</v>
+    <row r="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
@@ -516,7 +613,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>11</v>
@@ -524,17 +621,23 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
@@ -542,7 +645,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>11</v>
@@ -550,147 +653,322 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lots of merge fixes and some other stuff
</commit_message>
<xml_diff>
--- a/Need to be Merged.xlsx
+++ b/Need to be Merged.xlsx
@@ -8,12 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dante\Documents\Paradox Interactive\Hearts of Iron IV\mod\1984DEV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716737A4-3C1D-4F77-B89A-1ED919B1FE23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2F0312-D9FE-431C-9457-6831FAE64558}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3990" yWindow="1110" windowWidth="26085" windowHeight="13110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="825" yWindow="1245" windowWidth="26070" windowHeight="13110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Merge" sheetId="1" r:id="rId1"/>
+    <sheet name="Problems" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="275">
   <si>
     <t>industry.txt</t>
   </si>
@@ -243,13 +249,628 @@
   </si>
   <si>
     <t>REPLACED</t>
+  </si>
+  <si>
+    <t>(P)</t>
+  </si>
+  <si>
+    <t>Issues</t>
+  </si>
+  <si>
+    <t>Duplicate Localizations (see Sheet 3)</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'PAL_neutrality_DEF' in: '\localisation\countries_l_english.yml' at line 1125 and in: '\localisation\countries_l_english.yml' at line 1126</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_drums_of_war' in: '\localisation\nef_focus_resistance_l_english.yml' at line 26 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 267</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_our_countrys_pride' in: '\localisation\nef_focus_resistance_l_english.yml' at line 30 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 269</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_strength_through_sacrifice' in: '\localisation\nef_focus_resistance_l_english.yml' at line 113 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 271</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_equal_opportunity' in: '\localisation\nef_focus_resistance_l_english.yml' at line 33 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 274</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_beans_and_bullets' in: '\localisation\nef_focus_resistance_l_english.yml' at line 112 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 278</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_desperate_times' in: '\localisation\nef_focus_resistance_l_english.yml' at line 34 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 279</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_state_capitalism' in: '\localisation\nef_focus_resistance_l_english.yml' at line 106 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 280</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_final_indoctrination' in: '\localisation\nef_focus_resistance_l_english.yml' at line 117 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 282</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_desperate_measures' in: '\localisation\nef_focus_resistance_l_english.yml' at line 35 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 283</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_nuclear_reproliferation' in: '\localisation\nef_focus_resistance_l_english.yml' at line 125 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 284</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_unpaid_overtime' in: '\localisation\nef_focus_resistance_l_english.yml' at line 109 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 285</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_depleted_uranium' in: '\localisation\nef_focus_resistance_l_english.yml' at line 126 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 287</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_unrestricted_armaments' in: '\localisation\nef_focus_resistance_l_english.yml' at line 127 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 289</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_high_on_violence' in: '\localisation\nef_focus_resistance_l_english.yml' at line 128 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 291</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_our_countrys_pride_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 159 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 295</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_strength_through_sacrifice_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 234 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 297</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_equal_opportunity_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 162 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 300</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_beans_and_bullets_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 233 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 304</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_desperate_times_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 163 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 305</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_state_capitalism_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 227 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 307</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_final_indoctrination_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 238 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 309</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_desperate_measures_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 164 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 310</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_nuclear_reproliferation_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 246 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 311</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_unpaid_overtime_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 230 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 312</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_depleted_uranium_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 247 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 314</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_unrestricted_armaments_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 248 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 316</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_high_on_violence_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 249 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 318</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_equipment_effort' in: '\localisation\nef_focus_resistance_l_english.yml' at line 324 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 410</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_equipment_effort_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 325 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 411</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_motorization_effort' in: '\localisation\nef_focus_resistance_l_english.yml' at line 326 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 412</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_motorization_effort_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 327 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 413</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_doctrine_effort' in: '\localisation\nef_focus_resistance_l_english.yml' at line 328 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 414</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_doctrine_effort_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 329 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 415</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_equipment_effort_2' in: '\localisation\nef_focus_resistance_l_english.yml' at line 330 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 416</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_equipment_effort_2_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 331 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 417</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_mechanization_effort' in: '\localisation\nef_focus_resistance_l_english.yml' at line 332 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 418</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_mechanization_effort_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 333 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 419</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_doctrine_effort_2' in: '\localisation\nef_focus_resistance_l_english.yml' at line 334 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 420</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_doctrine_effort_2_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 335 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 421</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_equipment_effort_3' in: '\localisation\nef_focus_resistance_l_english.yml' at line 336 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 422</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_equipment_effort_3_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 337 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 423</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_armor_effort' in: '\localisation\nef_focus_resistance_l_english.yml' at line 338 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 424</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_armor_effort_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 339 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 425</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_special_forces' in: '\localisation\nef_focus_resistance_l_english.yml' at line 340 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 426</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_special_forces_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 341 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 427</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_hostile_environments' in: '\localisation\nef_focus_resistance_l_english.yml' at line 342 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 428</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_hostile_environments_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 343 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 429</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_aviation_effort' in: '\localisation\nef_focus_resistance_l_english.yml' at line 344 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 430</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_aviation_effort_tt' in: '\localisation\nef_focus_resistance_l_english.yml' at line 345 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 431</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_aviation_effort_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 346 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 432</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_fighter_focus' in: '\localisation\nef_focus_resistance_l_english.yml' at line 347 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 433</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_fighter_focus_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 348 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 434</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_bomber_focus' in: '\localisation\nef_focus_resistance_l_english.yml' at line 349 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 435</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_bomber_focus_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 350 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 436</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_aviation_effort_2' in: '\localisation\nef_focus_resistance_l_english.yml' at line 351 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 437</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_aviation_effort_2_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 352 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 438</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_CAS_effort' in: '\localisation\nef_focus_resistance_l_english.yml' at line 353 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 439</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_CAS_effort_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 354 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 440</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_rocket_effort' in: '\localisation\nef_focus_resistance_l_english.yml' at line 355 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 441</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_rocket_effort_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 356 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 442</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_NAV_effort' in: '\localisation\nef_focus_resistance_l_english.yml' at line 357 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 443</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_NAV_effort_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 358 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 444</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_naval_effort' in: '\localisation\nef_focus_resistance_l_english.yml' at line 359 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 445</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_naval_effort_tt' in: '\localisation\nef_focus_resistance_l_english.yml' at line 360 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 446</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_naval_effort_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 361 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 447</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_flexible_navy' in: '\localisation\nef_focus_resistance_l_english.yml' at line 362 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 448</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_flexible_navy_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 363 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 449</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_large_navy' in: '\localisation\nef_focus_resistance_l_english.yml' at line 364 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 450</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_large_navy_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 365 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 451</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_submarine_effort' in: '\localisation\nef_focus_resistance_l_english.yml' at line 366 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 452</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_submarine_effort_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 367 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 453</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_cruiser_effort' in: '\localisation\nef_focus_resistance_l_english.yml' at line 368 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 454</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_cruiser_effort_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 369 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 455</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_destroyer_effort' in: '\localisation\nef_focus_resistance_l_english.yml' at line 370 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 456</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_destroyer_effort_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 371 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 457</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_capital_ships_effort' in: '\localisation\nef_focus_resistance_l_english.yml' at line 372 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 458</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_capital_ships_effort_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 373 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 459</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_industrial_effort' in: '\localisation\nef_focus_resistance_l_english.yml' at line 374 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 460</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_industrial_effort_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 375 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 461</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_industrial_effort_2' in: '\localisation\nef_focus_resistance_l_english.yml' at line 376 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 462</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_industrial_effort_2_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 377 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 463</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_construction_effort' in: '\localisation\nef_focus_resistance_l_english.yml' at line 378 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 464</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_construction_effort_tt' in: '\localisation\nef_focus_resistance_l_english.yml' at line 379 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 465</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_construction_effort_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 380 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 466</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_production_effort' in: '\localisation\nef_focus_resistance_l_english.yml' at line 381 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 467</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_production_effort_tt' in: '\localisation\nef_focus_resistance_l_english.yml' at line 382 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 468</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_production_effort_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 383 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 469</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_construction_effort_2' in: '\localisation\nef_focus_resistance_l_english.yml' at line 384 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 470</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_construction_effort_2_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 385 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 471</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_production_effort_2' in: '\localisation\nef_focus_resistance_l_english.yml' at line 386 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 472</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_production_effort_2_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 387 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 473</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_production_effort_3' in: '\localisation\nef_focus_resistance_l_english.yml' at line 388 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 474</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_production_effort_3_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 389 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 475</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_infrastructure_effort' in: '\localisation\nef_focus_resistance_l_english.yml' at line 390 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 476</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_infrastructure_effort_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 391 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 477</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_infrastructure_effort_tt' in: '\localisation\nef_focus_resistance_l_english.yml' at line 392 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 478</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_synth_oil_effort_tt' in: '\localisation\nef_focus_resistance_l_english.yml' at line 393 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 479</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_infrastructure_effort_2' in: '\localisation\nef_focus_resistance_l_english.yml' at line 394 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 480</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_infrastructure_effort_2_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 395 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 481</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_construction_effort_3' in: '\localisation\nef_focus_resistance_l_english.yml' at line 396 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 482</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_construction_effort_3_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 397 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 483</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_nuclear_effort' in: '\localisation\nef_focus_resistance_l_english.yml' at line 398 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 484</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_nuclear_effort_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 399 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 485</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_secret_weapons' in: '\localisation\nef_focus_resistance_l_english.yml' at line 400 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 486</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_secret_weapons_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 401 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 487</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_air_innovation' in: '\localisation\nef_focus_resistance_l_english.yml' at line 402 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 488</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_air_innovation_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 403 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 489</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_air_innovation_2' in: '\localisation\nef_focus_resistance_l_english.yml' at line 404 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 490</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_air_innovation_2_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 405 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 491</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_naval_air_effort' in: '\localisation\nef_focus_resistance_l_english.yml' at line 406 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 492</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_res_naval_air_effort_desc' in: '\localisation\nef_focus_resistance_l_english.yml' at line 407 and in: '\localisation\nef_focus_resistance_l_english.yml' at line 493</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_threat_drumwar' in: '\localisation\nef_focus_resistance_l_english.yml' at line 2 and in: '\localisation\nef_focus_totalitarian_l_english.yml' at line 8</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_threat_decindep' in: '\localisation\nef_focus_resistance_l_english.yml' at line 3 and in: '\localisation\nef_focus_totalitarian_l_english.yml' at line 9</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_threat_domearth' in: '\localisation\nef_focus_resistance_l_english.yml' at line 4 and in: '\localisation\nef_focus_totalitarian_l_english.yml' at line 10</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_threat_liberateoceania' in: '\localisation\nef_focus_resistance_l_english.yml' at line 5 and in: '\localisation\nef_focus_totalitarian_l_english.yml' at line 11</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_threat_liberateeurasia' in: '\localisation\nef_focus_resistance_l_english.yml' at line 6 and in: '\localisation\nef_focus_totalitarian_l_english.yml' at line 12</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_threat_liberateeastasia' in: '\localisation\nef_focus_resistance_l_english.yml' at line 7 and in: '\localisation\nef_focus_totalitarian_l_english.yml' at line 13</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'ma_focus_tooltip' in: '\localisation\nef_focus_resistance_l_english.yml' at line 63 and in: '\localisation\nef_focus_totalitarian_l_english.yml' at line 60</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'gbp_focus_tooltip' in: '\localisation\nef_focus_resistance_l_english.yml' at line 64 and in: '\localisation\nef_focus_totalitarian_l_english.yml' at line 61</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'sf_focus_tooltip' in: '\localisation\nef_focus_resistance_l_english.yml' at line 65 and in: '\localisation\nef_focus_totalitarian_l_english.yml' at line 62</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'mw_focus_tooltip' in: '\localisation\nef_focus_resistance_l_english.yml' at line 66 and in: '\localisation\nef_focus_totalitarian_l_english.yml' at line 63</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'ci_focus_tooltip' in: '\localisation\nef_focus_resistance_l_english.yml' at line 67 and in: '\localisation\nef_focus_totalitarian_l_english.yml' at line 64</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'fib_focus_tooltip' in: '\localisation\nef_focus_resistance_l_english.yml' at line 68 and in: '\localisation\nef_focus_totalitarian_l_english.yml' at line 65</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'bs_focus_tooltip' in: '\localisation\nef_focus_resistance_l_english.yml' at line 69 and in: '\localisation\nef_focus_totalitarian_l_english.yml' at line 66</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'airdoc_focus_tooltip' in: '\localisation\nef_focus_resistance_l_english.yml' at line 70 and in: '\localisation\nef_focus_totalitarian_l_english.yml' at line 67</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_atomic_research_tt' in: '\localisation\nef_focus_resistance_l_english.yml' at line 319 and in: '\localisation\nef_focus_totalitarian_l_english.yml' at line 251</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_totalitarian_focus' in: '\localisation\nef_focus_resistance_l_english.yml' at line 320 and in: '\localisation\nef_focus_totalitarian_l_english.yml' at line 252</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'nef_ocp_desc' in: '\localisation\nef_ideas_l_english.yml' at line 211 and in: '\localisation\nef_ideas_l_english.yml' at line 213</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'military_theorist' in: '\localisation\nef_ideas_l_english.yml' at line 90 and in: '\localisation\traits_l_english.yml' at line 36</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'air_warfare_theorist' in: '\localisation\nef_ideas_l_english.yml' at line 91 and in: '\localisation\traits_l_english.yml' at line 37</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'naval_theorist' in: '\localisation\nef_ideas_l_english.yml' at line 92 and in: '\localisation\traits_l_english.yml' at line 42</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'tank_manufacturer' in: '\localisation\nef_ideas_l_english.yml' at line 66 and in: '\localisation\traits_l_english.yml' at line 46</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'naval_manufacturer' in: '\localisation\nef_ideas_l_english.yml' at line 67 and in: '\localisation\traits_l_english.yml' at line 51</t>
+  </si>
+  <si>
+    <t>Duplicated Loc: 'industrial_concern' in: '\localisation\nef_ideas_l_english.yml' at line 70 and in: '\localisation\traits_l_english.yml' at line 52</t>
+  </si>
+  <si>
+    <t>Untested</t>
+  </si>
+  <si>
+    <t>[20:01:42][persistent.cpp:52]: Error: "Unknown modifier: take_states_cost_factor, near line: 207" in file: "common/ideologies/00_ideologies.txt" near line: 207</t>
+  </si>
+  <si>
+    <t>[20:01:42][persistent.cpp:52]: Error: "Unknown modifier: research_time_factor, near line: 175" in file: "common/ideas/_economic.txt" near line: 175</t>
+  </si>
+  <si>
+    <t>[20:01:42][persistent.cpp:52]: Error: "Unknown modifier: research_time_factor, near line: 203" in file: "common/ideas/_economic.txt" near line: 203</t>
+  </si>
+  <si>
+    <t>[20:01:42][persistent.cpp:52]: Error: "Unknown modifier: research_time_factor, near line: 237" in file: "common/ideas/_economic.txt" near line: 237</t>
+  </si>
+  <si>
+    <t>[20:01:42][persistent.cpp:52]: Error: "Unknown modifier: enemy_partisan_effect, near line: 37" in file: "common/ideas/_manpower.txt" near line: 37</t>
+  </si>
+  <si>
+    <t>[20:01:42][persistent.cpp:52]: Error: "Unknown modifier: enemy_partisan_effect, near line: 93" in file: "common/ideas/_manpower.txt" near line: 93</t>
+  </si>
+  <si>
+    <t>[20:01:42][persistent.cpp:52]: Error: "Unknown modifier: research_time_factor, near line: 247" in file: "common/ideas/_manpower.txt" near line: 247</t>
+  </si>
+  <si>
+    <t>[20:01:42][persistent.cpp:52]: Error: "Unknown modifier: research_time_factor, near line: 294" in file: "common/ideas/_manpower.txt" near line: 294</t>
+  </si>
+  <si>
+    <t>[20:01:42][persistent.cpp:52]: Error: "Unknown modifier: research_time_factor, near line: 344" in file: "common/ideas/_manpower.txt" near line: 344</t>
+  </si>
+  <si>
+    <t>[20:01:42][persistent.cpp:52]: Error: "Unknown modifier: enemy_partisan_effect, near line: 41" in file: "common/ideas/_manpower_res.txt" near line: 41</t>
+  </si>
+  <si>
+    <t>[20:01:42][persistent.cpp:52]: Error: "Unknown modifier: enemy_partisan_effect, near line: 100" in file: "common/ideas/_manpower_res.txt" near line: 100</t>
+  </si>
+  <si>
+    <t>[20:01:42][persistent.cpp:52]: Error: "Unknown modifier: research_time_factor, near line: 219" in file: "common/ideas/_manpower_res.txt" near line: 219</t>
+  </si>
+  <si>
+    <t>[20:01:42][persistent.cpp:52]: Error: "Unknown modifier: research_time_factor, near line: 268" in file: "common/ideas/_manpower_res.txt" near line: 268</t>
+  </si>
+  <si>
+    <t>[20:01:42][persistent.cpp:52]: Error: "Unknown modifier: research_time_factor, near line: 319" in file: "common/ideas/_manpower_res.txt" near line: 319</t>
+  </si>
+  <si>
+    <t>[20:01:42][persistent.cpp:52]: Error: "Unknown modifier: enemy_partisan_effect, near line: 29" in file: "common/ideas/_nefideas.txt" near line: 29</t>
+  </si>
+  <si>
+    <t>[20:01:42][persistent.cpp:52]: Error: "Unknown modifier: research_time_factor, near line: 187" in file: "common/ideas/_nefideas.txt" near line: 187</t>
+  </si>
+  <si>
+    <t>[20:01:42][persistent.cpp:52]: Error: "Unknown modifier: research_time_factor, near line: 269" in file: "common/ideas/_nefideas.txt" near line: 269</t>
+  </si>
+  <si>
+    <t>[20:01:42][persistent.cpp:52]: Error: "Unknown modifier: research_time_factor, near line: 389" in file: "common/ideas/_nefideas.txt" near line: 389</t>
+  </si>
+  <si>
+    <t>[20:01:42][persistent.cpp:52]: Error: "Unknown modifier: research_time_factor, near line: 555" in file: "common/ideas/_nefideas.txt" near line: 555</t>
+  </si>
+  <si>
+    <t>[20:01:42][persistent.cpp:52]: Error: "Unknown modifier: naval_torpedo_range_factor, near line: 481" in file: "common/ideas/_nefideas_focus.txt" near line: 481</t>
+  </si>
+  <si>
+    <t>[20:01:42][persistent.cpp:52]: Error: "Unknown modifier: enemy_partisan_effect, near line: 1128" in file: "common/ideas/_nefideas_focus.txt" near line: 1128</t>
+  </si>
+  <si>
+    <t>[20:01:42][persistent.cpp:52]: Error: "Unknown modifier: enemy_partisan_effect, near line: 1201" in file: "common/ideas/_nefideas_focus.txt" near line: 1201</t>
+  </si>
+  <si>
+    <t>[20:01:42][persistent.cpp:52]: Error: "Unknown modifier: enemy_partisan_effect, near line: 1239" in file: "common/ideas/_nefideas_focus.txt" near line: 1239</t>
+  </si>
+  <si>
+    <t>[20:01:43][persistent.cpp:52]: Error: "Unknown modifier: partisan_effect, near line: 37" in file: "common/country_leader/01_neftraits.txt" near line: 37</t>
+  </si>
+  <si>
+    <t>[20:01:43][persistent.cpp:52]: Error: "Unknown modifier: enemy_partisan_effect, near line: 100" in file: "common/country_leader/01_neftraits.txt" near line: 100</t>
+  </si>
+  <si>
+    <t>[20:01:43][persistent.cpp:52]: Error: "Unknown modifier: research_time_factor, near line: 111" in file: "common/country_leader/01_neftraits.txt" near line: 111</t>
+  </si>
+  <si>
+    <t>[20:01:43][persistent.cpp:52]: Error: "Unknown modifier: research_time_factor, near line: 123" in file: "common/country_leader/01_neftraits.txt" near line: 123</t>
+  </si>
+  <si>
+    <t>[20:01:43][persistent.cpp:52]: Error: "Unknown modifier: enemy_partisan_effect, near line: 146" in file: "common/country_leader/01_neftraits.txt" near line: 146</t>
+  </si>
+  <si>
+    <t>[20:01:43][persistent.cpp:52]: Error: "Unexpected token: air_defense, near line: 297" in file: "common/country_leader/01_neftraits.txt" near line: 297</t>
+  </si>
+  <si>
+    <t>[20:01:43][persistent.cpp:52]: Error: "Unexpected token: air_defense, near line: 300" in file: "common/country_leader/01_neftraits.txt" near line: 300</t>
+  </si>
+  <si>
+    <t>[20:01:43][persistent.cpp:52]: Error: "Unexpected token: air_defense, near line: 303" in file: "common/country_leader/01_neftraits.txt" near line: 303</t>
+  </si>
+  <si>
+    <t>[20:01:43][persistent.cpp:52]: Error: "Unexpected token: air_defense, near line: 306" in file: "common/country_leader/01_neftraits.txt" near line: 306</t>
+  </si>
+  <si>
+    <t>[20:01:43][persistent.cpp:52]: Error: "Unexpected token: air_defense, near line: 309" in file: "common/country_leader/01_neftraits.txt" near line: 309</t>
+  </si>
+  <si>
+    <t>Incorrect Modifiers in Focus Trees (Sheet 4)</t>
+  </si>
+  <si>
+    <t>The vp 197 on line 24 of C:\Users\Dante\Documents\Paradox Interactive\Hearts of Iron IV\mod\1984DEV\history\states\147-Salla.txt does not have any localization.</t>
+  </si>
+  <si>
+    <t>The vp 12994 on line 27 of C:\Users\Dante\Documents\Paradox Interactive\Hearts of Iron IV\mod\1984DEV\history\states\506-Northern Chile.txt does not have any localization.</t>
+  </si>
+  <si>
+    <t>The vp 13067 on line 12 of C:\Users\Dante\Documents\Paradox Interactive\Hearts of Iron IV\mod\1984DEV\history\states\650-Attu Island.txt does not have any localization.</t>
+  </si>
+  <si>
+    <t>The vp localization 1827 on line 363 of C:\Users\Dante\Documents\Paradox Interactive\Hearts of Iron IV\mod\1984DEV\localisation\victory_points_l_english.yml does not have any corresponding victory point.</t>
+  </si>
+  <si>
+    <t>The vp localization 7302 on line 476 of C:\Users\Dante\Documents\Paradox Interactive\Hearts of Iron IV\mod\1984DEV\localisation\victory_points_l_english.yml does not have any corresponding victory point.</t>
+  </si>
+  <si>
+    <t>The vp localization 10367 on line 544 of C:\Users\Dante\Documents\Paradox Interactive\Hearts of Iron IV\mod\1984DEV\localisation\victory_points_l_english.yml does not have any corresponding victory point.</t>
+  </si>
+  <si>
+    <t>C:\Users\Dante\Documents\Paradox Interactive\Hearts of Iron IV\mod\1984DEV\common\defines\00_defines.lua Brackets: Expecting: '}' but found ')' around line 179</t>
+  </si>
+  <si>
+    <t>C:\Users\Dante\Documents\Paradox Interactive\Hearts of Iron IV\mod\1984DEV\common\defines\00_defines.lua Brackets: Not expected ')' around line 179</t>
+  </si>
+  <si>
+    <t>C:\Users\Dante\Documents\Paradox Interactive\Hearts of Iron IV\mod\1984DEV\common\defines\00_defines.lua Brackets: Not expected ')' around line 180</t>
+  </si>
+  <si>
+    <t>C:\Users\Dante\Documents\Paradox Interactive\Hearts of Iron IV\mod\1984DEV\common\defines\00_defines.lua Brackets: Not expected ')' around line 181</t>
+  </si>
+  <si>
+    <t>C:\Users\Dante\Documents\Paradox Interactive\Hearts of Iron IV\mod\1984DEV\common\defines\00_defines.lua Brackets: Not expected '}' around line 357</t>
+  </si>
+  <si>
+    <t>C:\Users\Dante\Documents\Paradox Interactive\Hearts of Iron IV\mod\1984DEV\common\defines\00_defines.lua Brackets: Expecting: ')' but found '}' around line 2407</t>
+  </si>
+  <si>
+    <t>C:\Users\Dante\Documents\Paradox Interactive\Hearts of Iron IV\mod\1984DEV\common\defines\00_defines.lua Brackets: Expecting: ']' but found ')' around line 2457</t>
+  </si>
+  <si>
+    <t>C:\Users\Dante\Documents\Paradox Interactive\Hearts of Iron IV\mod\1984DEV\common\defines\00_defines.lua Brackets: Expecting: ')' but found '}' around line 2566</t>
+  </si>
+  <si>
+    <t>C:\Users\Dante\Documents\Paradox Interactive\Hearts of Iron IV\mod\1984DEV\common\defines\00_defines.lua Brackets: Expecting: ')' but found '}' around line 2989</t>
+  </si>
+  <si>
+    <t>C:\Users\Dante\Documents\Paradox Interactive\Hearts of Iron IV\mod\1984DEV\common\defines\00_defines.lua Brackets: there are 2 opening bracket(s) without closing bracket(s)</t>
+  </si>
+  <si>
+    <t>Lua Syntax Issues (Sheet 6)</t>
+  </si>
+  <si>
+    <t>Bad VP loc  (Sheet 5)</t>
+  </si>
+  <si>
+    <t>C:\Users\Dante\Documents\Paradox Interactive\Hearts of Iron IV\mod\1984DEV\common\national_focus\nef_nf_nerd.txt Brackets: Not expected '}' around line 32</t>
+  </si>
+  <si>
+    <t>C:\Users\Dante\Documents\Paradox Interactive\Hearts of Iron IV\mod\1984DEV\common\units\names_divisions\BRA_names_divisions.txt Brackets: there are 1 opening bracket(s) without closing bracket(s)</t>
+  </si>
+  <si>
+    <t>C:\Users\Dante\Documents\Paradox Interactive\Hearts of Iron IV\mod\1984DEV\history\states\762-Silesian Voivodeship.txt Brackets: there are 1 opening bracket(s) without closing bracket(s)</t>
+  </si>
+  <si>
+    <t>Bad Syntax (Sheet 7)</t>
+  </si>
+  <si>
+    <t>Common Files</t>
+  </si>
+  <si>
+    <t>_nefideas_decisions.txt</t>
+  </si>
+  <si>
+    <t>_nefideas_focus.txt</t>
+  </si>
+  <si>
+    <t>_nefministers.txt</t>
+  </si>
+  <si>
+    <t>_economic.txt</t>
+  </si>
+  <si>
+    <t>_event.txt</t>
+  </si>
+  <si>
+    <t>_manpower.txt</t>
+  </si>
+  <si>
+    <t>_manpower_res.txt</t>
+  </si>
+  <si>
+    <t>_nefideas.txt</t>
+  </si>
+  <si>
+    <t>Doesn't Break</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,8 +884,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -301,6 +929,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -314,14 +960,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -602,10 +1251,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B68"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,11 +1441,17 @@
       <c r="A25" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="B25" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="B26" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
@@ -815,53 +1470,71 @@
       <c r="A29" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="B29" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="B30" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="B31" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>36</v>
       </c>
@@ -869,7 +1542,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>37</v>
       </c>
@@ -877,7 +1550,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>38</v>
       </c>
@@ -885,7 +1558,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>39</v>
       </c>
@@ -893,36 +1566,41 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B46" s="5"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B47" s="5"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -930,6 +1608,9 @@
       <c r="A49" s="4" t="s">
         <v>46</v>
       </c>
+      <c r="B49" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
@@ -974,7 +1655,7 @@
       <c r="A56" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="7" t="s">
         <v>68</v>
       </c>
     </row>
@@ -982,7 +1663,7 @@
       <c r="A57" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="7" t="s">
         <v>68</v>
       </c>
     </row>
@@ -990,7 +1671,7 @@
       <c r="A58" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B58" s="7" t="s">
         <v>68</v>
       </c>
     </row>
@@ -998,7 +1679,7 @@
       <c r="A59" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="B59" s="7" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1006,7 +1687,7 @@
       <c r="A60" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B60" s="7" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1014,7 +1695,7 @@
       <c r="A61" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B61" s="7" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1022,7 +1703,7 @@
       <c r="A62" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="B62" s="7" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1030,7 +1711,7 @@
       <c r="A63" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B63" s="7" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1038,7 +1719,7 @@
       <c r="A64" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B64" s="7" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1046,7 +1727,7 @@
       <c r="A65" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="B65" s="7" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1054,6 +1735,7 @@
       <c r="A66" s="4" t="s">
         <v>63</v>
       </c>
+      <c r="B66" s="5"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
@@ -1066,10 +1748,2219 @@
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>65</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9E4EFAD-B333-4BB1-ABFE-570333890F52}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.5703125" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCF59141-B160-400B-9E08-0268197489C2}">
+  <dimension ref="A1:C135"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B132" sqref="B132"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="170.85546875" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B135" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0354AE90-E777-4CBC-86F9-DA649DAB175D}">
+  <dimension ref="A1:C33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="142" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E13A48-B5BD-4490-9D36-803AD220A9D1}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="184.5703125" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>248</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2314EAB2-4E80-46D5-849F-42111D7637EE}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="162.42578125" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B0EDD5E-7A16-4038-8764-4E69A192941E}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="184.28515625" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Last of the localization and gui fixes
</commit_message>
<xml_diff>
--- a/Need to be Merged.xlsx
+++ b/Need to be Merged.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dante\Documents\Paradox Interactive\Hearts of Iron IV\mod\1984DEV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2F0312-D9FE-431C-9457-6831FAE64558}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C304ED57-0F5C-4246-AFAA-DF165EB4025C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="1245" windowWidth="26070" windowHeight="13110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="915" yWindow="1110" windowWidth="26070" windowHeight="13110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Merge" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="276">
   <si>
     <t>industry.txt</t>
   </si>
@@ -864,6 +864,9 @@
   </si>
   <si>
     <t>Doesn't Break</t>
+  </si>
+  <si>
+    <t>UNSURE IF ISSUE</t>
   </si>
 </sst>
 </file>
@@ -960,7 +963,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -971,6 +974,7 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1253,8 +1257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1405,6 +1409,9 @@
       <c r="A19" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="B19" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
@@ -1418,6 +1425,9 @@
       <c r="A21" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="B21" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
@@ -1431,11 +1441,17 @@
       <c r="A23" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="B23" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="B24" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
@@ -1465,6 +1481,9 @@
       <c r="A28" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="B28" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
@@ -1518,16 +1537,25 @@
       <c r="A35" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="B35" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="B36" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="B37" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="38" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
@@ -1570,28 +1598,41 @@
       <c r="A43" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="B43" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>41</v>
       </c>
+      <c r="B44" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>42</v>
       </c>
+      <c r="B45" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="5"/>
+      <c r="B46" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="5"/>
+      <c r="B47" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
@@ -1604,7 +1645,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>46</v>
       </c>
@@ -1612,20 +1653,26 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>49</v>
       </c>
@@ -1633,17 +1680,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>52</v>
       </c>
@@ -1651,7 +1704,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>53</v>
       </c>
@@ -1659,7 +1712,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>54</v>
       </c>
@@ -1667,7 +1720,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>55</v>
       </c>
@@ -1675,7 +1728,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>56</v>
       </c>
@@ -1683,7 +1736,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>57</v>
       </c>
@@ -1691,7 +1744,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>58</v>
       </c>
@@ -1699,7 +1752,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>59</v>
       </c>
@@ -1707,7 +1760,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>60</v>
       </c>
@@ -1715,7 +1768,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>61</v>
       </c>
@@ -1735,7 +1788,9 @@
       <c r="A66" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B66" s="5"/>
+      <c r="B66" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
@@ -1833,7 +1888,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1866,10 +1921,16 @@
       <c r="A4" s="6" t="s">
         <v>259</v>
       </c>
+      <c r="B4" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>260</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3771,10 +3832,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E13A48-B5BD-4490-9D36-803AD220A9D1}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,35 +3843,38 @@
     <col min="1" max="1" width="184.5703125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" s="10"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" s="10"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>248</v>
       </c>
+      <c r="B6" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Pulled in base map
</commit_message>
<xml_diff>
--- a/Need to be Merged.xlsx
+++ b/Need to be Merged.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dante\Documents\Paradox Interactive\Hearts of Iron IV\mod\1984DEV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C304ED57-0F5C-4246-AFAA-DF165EB4025C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F2A43A-937F-4874-87D4-93DD745FEEA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="1110" windowWidth="26070" windowHeight="13110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1815" yWindow="1845" windowWidth="26070" windowHeight="13110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Merge" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="276">
   <si>
     <t>industry.txt</t>
   </si>
@@ -1257,8 +1257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1630,9 +1630,7 @@
       <c r="A47" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>68</v>
-      </c>
+      <c r="B47" s="2"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
@@ -1805,7 +1803,7 @@
         <v>65</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
     </row>
     <row r="69" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pulled in graphics and icons
</commit_message>
<xml_diff>
--- a/Need to be Merged.xlsx
+++ b/Need to be Merged.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dante\Documents\Paradox Interactive\Hearts of Iron IV\mod\1984DEV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F2A43A-937F-4874-87D4-93DD745FEEA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E43E14-7FA5-4C78-B25D-816BB608CF9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="1845" windowWidth="26070" windowHeight="13110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="1500" windowWidth="26070" windowHeight="13110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Merge" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="276">
   <si>
     <t>industry.txt</t>
   </si>
@@ -1257,8 +1257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1630,7 +1630,9 @@
       <c r="A47" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="2"/>
+      <c r="B47" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">

</xml_diff>